<commit_message>
allows overwriting common parameters
</commit_message>
<xml_diff>
--- a/spreadsheet_conversion/many_subjects_sheet/subjects_metadata_example.xlsx
+++ b/spreadsheet_conversion/many_subjects_sheet/subjects_metadata_example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BIDS\ONP\BIDS-converter\spreadsheet_conversion\many_subjects_sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB61C57-D5D7-46A2-A40F-986F1F760E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5643DE6-19B6-445B-859D-F3D36DE1633B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{B09AB50C-E81C-BF4B-AB80-4C0F8EC55ACD}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>InjectedRadioactivity</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>D:\BIDS\ONP\BIDS-converter\spreadsheet_conversion\many_subjects_sheet\sub-09\pet</t>
+  </si>
+  <si>
+    <t>FrameTimesStart</t>
+  </si>
+  <si>
+    <t>FrameDuration</t>
+  </si>
+  <si>
+    <t>0,10,20,30,40,50,60,80,100,120,140,160,180,240,310,360,420,480,540,660,780,900,1020,1140,1260,1380,1500,1800,2100,2400,2700,3000,3300,3600,3900,4200,4500,4800,5100,5400,5700,6000,6300,6600,6900</t>
+  </si>
+  <si>
+    <t>10,10,10,10,10,10,20,20,20,20,20,20,60,60,50,60,60,60,120,120,120,120,120,120,120,120,300,300,300,300,300,300,300,300,300,300,300,300,300,300,300,300,300,300,300</t>
   </si>
 </sst>
 </file>
@@ -136,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -150,6 +162,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -465,23 +481,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D07A739-95C2-BD46-B2B0-50E40D980EB4}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="71.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.9140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="255.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="83.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.4140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.08203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.4140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.58203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.58203125" customWidth="1"/>
+    <col min="7" max="7" width="28.58203125" customWidth="1"/>
+    <col min="8" max="8" width="33.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -500,8 +518,14 @@
       <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -517,11 +541,15 @@
       <c r="E2" s="5">
         <v>0.57100694444444444</v>
       </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F2" s="7"/>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -537,8 +565,9 @@
       <c r="E3" s="5">
         <v>0.38347222222222221</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -554,8 +583,11 @@
       <c r="E4" s="5">
         <v>0.46880787037037036</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F4" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -571,8 +603,9 @@
       <c r="E5" s="5">
         <v>0.65688657407407403</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -588,8 +621,9 @@
       <c r="E6" s="5">
         <v>0.67562500000000003</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -605,8 +639,9 @@
       <c r="E7" s="5">
         <v>0.50001157407407404</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -622,8 +657,9 @@
       <c r="E8" s="5">
         <v>0.42714120370370368</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -639,8 +675,9 @@
       <c r="E9" s="5">
         <v>0.42541666666666672</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -656,6 +693,7 @@
       <c r="E10" s="5">
         <v>0.60116898148148146</v>
       </c>
+      <c r="F10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>